<commit_message>
some new aux methods
</commit_message>
<xml_diff>
--- a/data/waffen.xlsx
+++ b/data/waffen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaelm\srh_proj_dsa\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SRH\Documents\GitHub\srh_proj_dsa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B0324C-AB59-4C84-B3E4-69086100F339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF527FC-55EC-432D-B9F2-62D9E4D5CE25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Art</t>
   </si>
@@ -90,10 +87,7 @@
     <t>Fechtwaffen</t>
   </si>
   <si>
-    <t>Vorteil</t>
-  </si>
-  <si>
-    <t>Nachteil</t>
+    <t>Waffe</t>
   </si>
 </sst>
 </file>
@@ -129,17 +123,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -417,59 +408,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="11" width="20.7109375" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="9" width="20.6640625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -478,7 +463,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1">
         <v>14</v>
@@ -490,16 +475,16 @@
         <v>-1</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
@@ -507,7 +492,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1">
         <v>14</v>
@@ -519,15 +504,15 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -536,7 +521,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1">
         <v>15</v>
@@ -548,15 +533,15 @@
         <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -565,7 +550,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="1">
         <v>15</v>
@@ -577,7 +562,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>